<commit_message>
Money Tracker deploy v1 - with swagger
</commit_message>
<xml_diff>
--- a/MoneyTracker/Helpers/Excel/SeedFiles/UserDetail.xlsx
+++ b/MoneyTracker/Helpers/Excel/SeedFiles/UserDetail.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IQ\Projects\NedBank\Code\Samples\MoneyTrackerPOCInMem\MoneyTrackerPOCInMem\DAL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IQ\Projects\NedBank\Code\BitBucket\dev\nedbank-money-tracker\MoneyTracker\MoneyTracker\Helpers\Excel\SeedFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA9FAFF2-59D1-4059-9E38-6100EF3AA4F3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51E577CA-F7EC-4D90-84F6-B604E5E2C3F7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CDE4DE60-7C19-4AA7-A04B-40BE9DEDAEB1}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8964" xr2:uid="{CDE4DE60-7C19-4AA7-A04B-40BE9DEDAEB1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t>UserDetailId</t>
   </si>
@@ -82,6 +82,30 @@
   </si>
   <si>
     <t>Test user GoTo BackTo OnlineBanking No Accounts</t>
+  </si>
+  <si>
+    <t>cisNumber</t>
+  </si>
+  <si>
+    <t>110001263706</t>
+  </si>
+  <si>
+    <t>110001263707</t>
+  </si>
+  <si>
+    <t>110001263708</t>
+  </si>
+  <si>
+    <t>110001263709</t>
+  </si>
+  <si>
+    <t>110001263710</t>
+  </si>
+  <si>
+    <t>110001263711</t>
+  </si>
+  <si>
+    <t>110001263712</t>
   </si>
 </sst>
 </file>
@@ -117,8 +141,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -433,174 +458,193 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBB62C34-8D6E-4598-BFF6-65ACA0D74B94}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
+      <c r="B1" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="b">
-        <v>0</v>
-      </c>
       <c r="E2" t="b">
         <v>0</v>
       </c>
       <c r="F2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" t="b">
-        <v>0</v>
-      </c>
       <c r="E3" t="b">
         <v>0</v>
       </c>
       <c r="F3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>13</v>
       </c>
-      <c r="D4" t="b">
-        <v>0</v>
-      </c>
       <c r="E4" t="b">
         <v>0</v>
       </c>
       <c r="F4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>4</v>
       </c>
-      <c r="D5" t="b">
-        <v>1</v>
-      </c>
       <c r="E5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
         <v>15</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>4</v>
       </c>
-      <c r="D6" t="b">
-        <v>0</v>
-      </c>
       <c r="E6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6" t="b">
         <v>1</v>
       </c>
       <c r="G6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="H6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
         <v>16</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>4</v>
       </c>
-      <c r="D7" t="b">
-        <v>0</v>
-      </c>
       <c r="E7" t="b">
         <v>0</v>
       </c>
@@ -608,29 +652,35 @@
         <v>0</v>
       </c>
       <c r="G7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="H7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
         <v>2</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>4</v>
       </c>
-      <c r="D8" t="b">
-        <v>0</v>
-      </c>
       <c r="E8" t="b">
         <v>0</v>
       </c>
       <c r="F8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>